<commit_message>
Multiple insance and Group chat remaining
</commit_message>
<xml_diff>
--- a/PushStartup-Skypebot/log/DB.xlsx
+++ b/PushStartup-Skypebot/log/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Campaign" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -44,7 +44,10 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>ConactSend</t>
+    <t>BotUserhandle</t>
+  </si>
+  <si>
+    <t>MessegeSend</t>
   </si>
 </sst>
 </file>
@@ -386,18 +389,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,13 +410,16 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
+      <c r="F1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -423,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>